<commit_message>
update test case home page
update test case home page
</commit_message>
<xml_diff>
--- a/Documents/FM_test case home page.xlsx
+++ b/Documents/FM_test case home page.xlsx
@@ -45,9 +45,6 @@
     <t>Status</t>
   </si>
   <si>
-    <t>check giao diện</t>
-  </si>
-  <si>
     <t>giao diện hiện lên website</t>
   </si>
   <si>
@@ -127,6 +124,9 @@
   </si>
   <si>
     <t>lúc đã làm xong đề thi</t>
+  </si>
+  <si>
+    <t>Check giao diện</t>
   </si>
 </sst>
 </file>
@@ -217,9 +217,6 @@
   <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -228,9 +225,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -239,27 +233,33 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -565,7 +565,7 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -585,7 +585,7 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -619,23 +619,23 @@
         <v>1</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1">
         <v>3</v>
       </c>
       <c r="G8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -643,24 +643,24 @@
         <f>A8+1</f>
         <v>2</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="D9" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>17</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1">
         <v>3</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="G9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" s="4" t="s">
         <v>12</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -668,22 +668,22 @@
         <f t="shared" ref="A10:A18" si="0">A9+1</f>
         <v>3</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="3" t="s">
+      <c r="B10" s="16"/>
+      <c r="C10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>19</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1">
         <v>3</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="G10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" s="4" t="s">
         <v>12</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -691,22 +691,22 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="3" t="s">
+      <c r="B11" s="16"/>
+      <c r="C11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>20</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>21</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1">
         <v>3</v>
       </c>
-      <c r="G11" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>22</v>
+      <c r="G11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -714,22 +714,22 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="9" t="s">
+      <c r="B12" s="16"/>
+      <c r="C12" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8">
-        <v>3</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H12" s="9" t="s">
-        <v>22</v>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6">
+        <v>3</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -737,24 +737,24 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="D13" s="5" t="s">
         <v>26</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>27</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1">
         <v>3</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="G13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H13" s="4" t="s">
         <v>12</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -762,20 +762,20 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="14" t="s">
-        <v>28</v>
+      <c r="B14" s="18"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="10" t="s">
+        <v>27</v>
       </c>
       <c r="E14" s="1"/>
-      <c r="F14" s="11">
-        <v>3</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H14" s="5" t="s">
-        <v>22</v>
+      <c r="F14" s="9">
+        <v>3</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -783,24 +783,24 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="D15" s="16" t="s">
-        <v>11</v>
+      <c r="D15" s="11" t="s">
+        <v>10</v>
       </c>
       <c r="E15" s="1"/>
-      <c r="F15" s="11">
-        <v>3</v>
-      </c>
-      <c r="G15" s="5" t="s">
+      <c r="F15" s="9">
+        <v>3</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H15" s="4" t="s">
         <v>12</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -808,20 +808,20 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B16" s="15"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="7" t="s">
-        <v>31</v>
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="5" t="s">
+        <v>30</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1">
         <v>3</v>
       </c>
-      <c r="G16" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H16" s="5" t="s">
-        <v>22</v>
+      <c r="G16" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -829,24 +829,24 @@
         <f>A16+1</f>
         <v>10</v>
       </c>
-      <c r="B17" s="13" t="s">
+      <c r="B17" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="D17" s="12" t="s">
         <v>33</v>
-      </c>
-      <c r="D17" s="18" t="s">
-        <v>34</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1">
         <v>3</v>
       </c>
-      <c r="G17" s="5" t="s">
+      <c r="G17" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H17" s="4" t="s">
         <v>12</v>
-      </c>
-      <c r="H17" s="5" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -854,22 +854,22 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B18" s="13"/>
+      <c r="B18" s="14"/>
       <c r="C18" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D18" s="18" t="s">
         <v>35</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>34</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1">
         <v>3</v>
       </c>
-      <c r="G18" s="19" t="s">
+      <c r="G18" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="H18" s="13" t="s">
         <v>12</v>
-      </c>
-      <c r="H18" s="19" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>